<commit_message>
Fix: standardized_IS updated (Published)
Figure from published filing showed different Net Income Loss due to the split of:
Net Income (loss) (operations)
Net Income (loss) to parent (incl. Non contr. Interest)
Now incorporated in the standardized_IS
Minor: update figures in output tables with 2 decimal digit
</commit_message>
<xml_diff>
--- a/data/standardized_IS.xlsx
+++ b/data/standardized_IS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/GitHub/R /SEC_data_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C1E512-FB85-F840-B3AD-1FBFFAE80CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDC7B85-894C-BB4D-B2D5-3E753736A8B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="500" windowWidth="21140" windowHeight="20020" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
+    <workbookView xWindow="4720" yWindow="1780" windowWidth="21140" windowHeight="20020" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="62">
   <si>
     <t>Revenue</t>
   </si>
@@ -155,9 +155,6 @@
     <t>NetIncomeLoss</t>
   </si>
   <si>
-    <t>Net Income (loss)</t>
-  </si>
-  <si>
     <t>Other Non Operating Income (Loss) Net</t>
   </si>
   <si>
@@ -219,6 +216,12 @@
   </si>
   <si>
     <t>Financial Report</t>
+  </si>
+  <si>
+    <t>Net Income (loss) (operations)</t>
+  </si>
+  <si>
+    <t>Net Income (loss) to parent (incl. Non contr. Interest)</t>
   </si>
 </sst>
 </file>
@@ -618,7 +621,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="A24:XFD60"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -632,19 +635,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -653,16 +656,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -671,16 +674,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -695,10 +698,10 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -712,10 +715,10 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -729,10 +732,10 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -746,10 +749,10 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -763,10 +766,10 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -780,10 +783,10 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -797,15 +800,15 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>29</v>
@@ -814,10 +817,10 @@
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -831,10 +834,10 @@
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -848,10 +851,10 @@
         <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -865,10 +868,10 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -882,10 +885,10 @@
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -899,10 +902,10 @@
         <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -910,16 +913,16 @@
         <v>34</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -927,16 +930,16 @@
         <v>34</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -944,16 +947,16 @@
         <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -961,16 +964,16 @@
         <v>34</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>51</v>
-      </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -984,44 +987,44 @@
         <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>